<commit_message>
Add and update analysis, physics, setup, and trajectory files
</commit_message>
<xml_diff>
--- a/Setup/LoadDimensions_ant.xlsx
+++ b/Setup/LoadDimensions_ant.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\AntsShapes\Setup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\Puzzle_collective_transport\Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3168" yWindow="192" windowWidth="14400" windowHeight="7356"/>
+    <workbookView xWindow="3170" yWindow="190" windowWidth="14400" windowHeight="7360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>LongI</t>
   </si>
 </sst>
 </file>
@@ -370,15 +373,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -406,7 +409,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -420,7 +423,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -434,7 +437,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -448,7 +451,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -460,6 +463,20 @@
       </c>
       <c r="D6">
         <v>1.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>1.75</v>
+      </c>
+      <c r="D7">
+        <v>1.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>